<commit_message>
Updated .gitignore Fixed so car rotates on the right point. Updated our progress on the burndownchart Added a second player
</commit_message>
<xml_diff>
--- a/doc/Game BurnDownChart.xlsx
+++ b/doc/Game BurnDownChart.xlsx
@@ -572,41 +572,41 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="126429824"/>
-        <c:axId val="126456192"/>
+        <c:axId val="84620800"/>
+        <c:axId val="84622336"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="126429824"/>
+        <c:axId val="84620800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126456192"/>
+        <c:crossAx val="84622336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="126456192"/>
+        <c:axId val="84622336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -614,7 +614,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126429824"/>
+        <c:crossAx val="84620800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -625,10 +625,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.7035820209973751"/>
-          <c:y val="0.43017169728783922"/>
+          <c:x val="0.70358202099737499"/>
+          <c:y val="0.43017169728783933"/>
           <c:w val="0.28934631459510268"/>
-          <c:h val="0.3136682590034181"/>
+          <c:h val="0.31366825900341816"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -637,7 +637,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -784,25 +784,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="70772224"/>
-        <c:axId val="70773760"/>
+        <c:axId val="87985536"/>
+        <c:axId val="88003712"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="70772224"/>
+        <c:axId val="87985536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70773760"/>
+        <c:crossAx val="88003712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="70773760"/>
+        <c:axId val="88003712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,7 +810,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70772224"/>
+        <c:crossAx val="87985536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -823,7 +823,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1399,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1693,16 +1693,16 @@
         <v>3</v>
       </c>
       <c r="H18" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K18" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="3:11">
@@ -1749,16 +1749,16 @@
         <v>2</v>
       </c>
       <c r="H20" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J20" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K20" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="3:11">
@@ -1807,16 +1807,16 @@
         <v>2</v>
       </c>
       <c r="H22" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J22" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K22" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="3:11">
@@ -1836,16 +1836,16 @@
         <v>5</v>
       </c>
       <c r="H23" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I23" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J23" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K23" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="3:11">
@@ -1971,19 +1971,19 @@
       </c>
       <c r="H28" s="13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I28" s="13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J28" s="13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K28" s="13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="3:11">
@@ -2020,7 +2020,7 @@
       </c>
       <c r="E33">
         <f>H28</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="3:5">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="E34">
         <f>I28</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="3:5">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="E35">
         <f>J28</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="3:5">
@@ -2059,7 +2059,7 @@
       </c>
       <c r="E36">
         <f>K28</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="3:5">

</xml_diff>

<commit_message>
Changed back so map has static bitmap Also updated burndownchart
Signed-off-by: Christoffer Johnsson <stoffe1992@hotmail.com>
</commit_message>
<xml_diff>
--- a/doc/Game BurnDownChart.xlsx
+++ b/doc/Game BurnDownChart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>Resouces</t>
   </si>
@@ -142,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,13 +176,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -426,7 +419,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1855,7 +1847,9 @@
       <c r="D24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="31"/>
+      <c r="E24" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="F24" s="17">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Merged cloud and info work
Signed-off-by: Christoffer Johnsson <stoffe1992@hotmail.com>
</commit_message>
<xml_diff>
--- a/doc/Game BurnDownChart.xlsx
+++ b/doc/Game BurnDownChart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>Resouces</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Fidde/Manne</t>
+  </si>
+  <si>
+    <t>Magnus</t>
   </si>
 </sst>
 </file>
@@ -567,38 +570,38 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84620800"/>
-        <c:axId val="84622336"/>
+        <c:axId val="91436544"/>
+        <c:axId val="91438080"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="84620800"/>
+        <c:axId val="91436544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84622336"/>
+        <c:crossAx val="91438080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="84622336"/>
+        <c:axId val="91438080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +609,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84620800"/>
+        <c:crossAx val="91436544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -617,10 +620,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.70358202099737499"/>
-          <c:y val="0.43017169728783933"/>
+          <c:x val="0.70358202099737477"/>
+          <c:y val="0.43017169728783955"/>
           <c:w val="0.28934631459510268"/>
-          <c:h val="0.31366825900341816"/>
+          <c:h val="0.31366825900341827"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -629,7 +632,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -776,25 +779,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87985536"/>
-        <c:axId val="88003712"/>
+        <c:axId val="93490560"/>
+        <c:axId val="93508736"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="87985536"/>
+        <c:axId val="93490560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88003712"/>
+        <c:crossAx val="93508736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="88003712"/>
+        <c:axId val="93508736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,7 +805,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87985536"/>
+        <c:crossAx val="93490560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -815,7 +818,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1391,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1513,7 +1516,7 @@
     </row>
     <row r="10" spans="3:11">
       <c r="F10" s="25" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="G10" s="6">
         <v>3</v>
@@ -1688,13 +1691,13 @@
         <v>2</v>
       </c>
       <c r="I18" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J18" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="3:11">
@@ -1704,7 +1707,9 @@
       <c r="D19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="17"/>
+      <c r="E19" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="F19" s="17">
         <v>1</v>
       </c>
@@ -1715,13 +1720,13 @@
         <v>1</v>
       </c>
       <c r="I19" s="17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J19" s="17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K19" s="17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="3:11">
@@ -1744,13 +1749,13 @@
         <v>1</v>
       </c>
       <c r="I20" s="17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J20" s="17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K20" s="17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="3:11">
@@ -1831,13 +1836,13 @@
         <v>3</v>
       </c>
       <c r="I23" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J23" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K23" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="3:11">
@@ -1860,13 +1865,13 @@
         <v>2</v>
       </c>
       <c r="I24" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="3:11">
@@ -1945,13 +1950,13 @@
         <v>6</v>
       </c>
       <c r="I27" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J27" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K27" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="3:11">
@@ -1969,15 +1974,15 @@
       </c>
       <c r="I28" s="13">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J28" s="13">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="K28" s="13">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="3:11">
@@ -2027,7 +2032,7 @@
       </c>
       <c r="E34">
         <f>I28</f>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="3:5">
@@ -2040,7 +2045,7 @@
       </c>
       <c r="E35">
         <f>J28</f>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="3:5">
@@ -2053,7 +2058,7 @@
       </c>
       <c r="E36">
         <f>K28</f>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="3:5">

</xml_diff>

<commit_message>
worked on menu and also added so something happens when you have done your laps
Signed-off-by: Christoffer Johnsson <stoffe1992@hotmail.com>
</commit_message>
<xml_diff>
--- a/doc/Game BurnDownChart.xlsx
+++ b/doc/Game BurnDownChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="2" r:id="rId1"/>
@@ -583,25 +583,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="91436544"/>
-        <c:axId val="91438080"/>
+        <c:axId val="82720256"/>
+        <c:axId val="82721792"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="91436544"/>
+        <c:axId val="82720256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91438080"/>
+        <c:crossAx val="82721792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="91438080"/>
+        <c:axId val="82721792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,7 +609,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91436544"/>
+        <c:crossAx val="82720256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -620,10 +620,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.70358202099737477"/>
-          <c:y val="0.43017169728783955"/>
+          <c:x val="0.70358202099737466"/>
+          <c:y val="0.43017169728783966"/>
           <c:w val="0.28934631459510268"/>
-          <c:h val="0.31366825900341827"/>
+          <c:h val="0.31366825900341833"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -632,7 +632,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -779,25 +779,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93490560"/>
-        <c:axId val="93508736"/>
+        <c:axId val="57642368"/>
+        <c:axId val="57660544"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="93490560"/>
+        <c:axId val="57642368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93508736"/>
+        <c:crossAx val="57660544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="93508736"/>
+        <c:axId val="57660544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,20 +805,21 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93490560"/>
+        <c:crossAx val="57642368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1394,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2075,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C21:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Created tests and created the menues
Signed-off-by: Christoffer Johnsson <stoffe1992@hotmail.com>
</commit_message>
<xml_diff>
--- a/doc/Game BurnDownChart.xlsx
+++ b/doc/Game BurnDownChart.xlsx
@@ -1017,25 +1017,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="94323840"/>
-        <c:axId val="94325376"/>
+        <c:axId val="83445248"/>
+        <c:axId val="83446784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="94323840"/>
+        <c:axId val="83445248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94325376"/>
+        <c:crossAx val="83446784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="94325376"/>
+        <c:axId val="83446784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,7 +1043,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94323840"/>
+        <c:crossAx val="83445248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1054,8 +1054,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.70358202099737432"/>
-          <c:y val="0.43017169728783994"/>
+          <c:x val="0.70358202099737421"/>
+          <c:y val="0.43017169728784005"/>
           <c:w val="0.28934631459510268"/>
           <c:h val="0.31366825900341838"/>
         </c:manualLayout>
@@ -1066,7 +1066,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1082,8 +1082,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.0652066016912475E-2"/>
-          <c:y val="8.9589878188303412E-2"/>
+          <c:x val="9.0652066016912503E-2"/>
+          <c:y val="8.9589878188303454E-2"/>
           <c:w val="0.50605584698953865"/>
           <c:h val="0.64173685981560002"/>
         </c:manualLayout>
@@ -1223,25 +1223,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="94526464"/>
-        <c:axId val="94552832"/>
+        <c:axId val="84974976"/>
+        <c:axId val="84984960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="94526464"/>
+        <c:axId val="84974976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94552832"/>
+        <c:crossAx val="84984960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="94552832"/>
+        <c:axId val="84984960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,7 +1249,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94526464"/>
+        <c:crossAx val="84974976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1263,7 +1263,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2639,8 +2639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C21:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
updated racegame and updated the burn down chart
Signed-off-by: Christoffer Johnsson <stoffe1992@hotmail.com>
</commit_message>
<xml_diff>
--- a/doc/Game BurnDownChart.xlsx
+++ b/doc/Game BurnDownChart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="72">
   <si>
     <t>Resouces</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Stoffe</t>
   </si>
   <si>
-    <t>Tobbe</t>
-  </si>
-  <si>
     <t>Mattias</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>CountDown</t>
   </si>
   <si>
-    <t>GameSound</t>
-  </si>
-  <si>
     <t>Game Sound</t>
   </si>
   <si>
@@ -165,15 +159,9 @@
     <t>Magnus/Tobias/Stoffe</t>
   </si>
   <si>
-    <t>Car collision</t>
-  </si>
-  <si>
     <t>Start position</t>
   </si>
   <si>
-    <t>Car collsion</t>
-  </si>
-  <si>
     <t>Övning 4 Manne</t>
   </si>
   <si>
@@ -223,6 +211,27 @@
   </si>
   <si>
     <t>Specialare:</t>
+  </si>
+  <si>
+    <t>Timer</t>
+  </si>
+  <si>
+    <t>Refaktorisera</t>
+  </si>
+  <si>
+    <t>Philip</t>
+  </si>
+  <si>
+    <t>Förbättra AI</t>
+  </si>
+  <si>
+    <t>Magnus/Fidde</t>
+  </si>
+  <si>
+    <t>Alla</t>
+  </si>
+  <si>
+    <t>Skriva in i XNA</t>
   </si>
 </sst>
 </file>
@@ -1017,25 +1026,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83445248"/>
-        <c:axId val="83446784"/>
+        <c:axId val="91899392"/>
+        <c:axId val="91900928"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="83445248"/>
+        <c:axId val="91899392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83446784"/>
+        <c:crossAx val="91900928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="83446784"/>
+        <c:axId val="91900928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,7 +1052,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83445248"/>
+        <c:crossAx val="91899392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1054,8 +1063,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.70358202099737421"/>
-          <c:y val="0.43017169728784005"/>
+          <c:x val="0.7035820209973741"/>
+          <c:y val="0.43017169728784022"/>
           <c:w val="0.28934631459510268"/>
           <c:h val="0.31366825900341838"/>
         </c:manualLayout>
@@ -1066,7 +1075,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1082,8 +1091,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.0652066016912503E-2"/>
-          <c:y val="8.9589878188303454E-2"/>
+          <c:x val="9.065206601691253E-2"/>
+          <c:y val="8.9589878188303496E-2"/>
           <c:w val="0.50605584698953865"/>
           <c:h val="0.64173685981560002"/>
         </c:manualLayout>
@@ -1204,44 +1213,44 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>26.5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84974976"/>
-        <c:axId val="84984960"/>
+        <c:axId val="92511616"/>
+        <c:axId val="92521600"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="84974976"/>
+        <c:axId val="92511616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84984960"/>
+        <c:crossAx val="92521600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="84984960"/>
+        <c:axId val="92521600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,7 +1258,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84974976"/>
+        <c:crossAx val="92511616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1263,7 +1272,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1624,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:D26"/>
+  <dimension ref="B4:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1639,13 +1648,13 @@
   <sheetData>
     <row r="4" spans="2:4">
       <c r="B4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -1653,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="10">
         <v>2</v>
@@ -1664,7 +1673,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="10">
         <v>2</v>
@@ -1675,7 +1684,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="10">
         <v>2</v>
@@ -1686,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="10">
         <v>4</v>
@@ -1697,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="10">
         <v>3</v>
@@ -1708,7 +1717,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="10">
         <v>4</v>
@@ -1719,7 +1728,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="10">
         <v>3</v>
@@ -1730,7 +1739,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="10">
         <v>2</v>
@@ -1741,7 +1750,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1752,7 +1761,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1761,7 +1770,7 @@
     <row r="15" spans="2:4" ht="18.75">
       <c r="B15" s="10"/>
       <c r="C15" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -1769,7 +1778,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1780,7 +1789,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1794,7 +1803,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1805,7 +1814,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -1816,7 +1825,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1827,7 +1836,7 @@
         <v>15</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1838,7 +1847,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1849,32 +1858,57 @@
         <v>17</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24">
         <v>1.5</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25">
-        <v>18</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
+      <c r="C25" s="14"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26">
         <v>19</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D26">
         <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28">
+        <v>21</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29">
+        <v>22</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1988,7 +2022,7 @@
     </row>
     <row r="9" spans="3:11">
       <c r="F9" s="51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="4">
         <v>3</v>
@@ -2008,7 +2042,7 @@
     </row>
     <row r="10" spans="3:11">
       <c r="F10" s="52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="4">
         <v>3</v>
@@ -2028,7 +2062,7 @@
     </row>
     <row r="11" spans="3:11">
       <c r="F11" s="53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" s="4">
         <v>3</v>
@@ -2048,7 +2082,7 @@
     </row>
     <row r="12" spans="3:11">
       <c r="F12" s="54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" s="4">
         <v>3</v>
@@ -2068,7 +2102,7 @@
     </row>
     <row r="13" spans="3:11">
       <c r="F13" s="56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G13" s="22">
         <v>3</v>
@@ -2111,22 +2145,22 @@
     </row>
     <row r="16" spans="3:11" ht="24" thickBot="1">
       <c r="C16" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="3:11" ht="15.75" thickBot="1">
       <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="60" t="s">
         <v>10</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>11</v>
       </c>
       <c r="G17" s="61">
         <v>41316</v>
@@ -2149,10 +2183,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="40">
         <v>3</v>
@@ -2178,10 +2212,10 @@
         <v>2</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="41">
         <v>1</v>
@@ -2207,10 +2241,10 @@
         <v>3</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" s="41">
         <v>2</v>
@@ -2236,10 +2270,10 @@
         <v>4</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="41">
         <v>2</v>
@@ -2265,10 +2299,10 @@
         <v>5</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" s="41">
         <v>2</v>
@@ -2294,10 +2328,10 @@
         <v>6</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F23" s="41">
         <v>5</v>
@@ -2323,10 +2357,10 @@
         <v>7</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" s="41">
         <v>2</v>
@@ -2352,10 +2386,10 @@
         <v>8</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F25" s="41">
         <v>0.5</v>
@@ -2381,7 +2415,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E26" s="35" t="s">
         <v>3</v>
@@ -2410,10 +2444,10 @@
         <v>10</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E27" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F27" s="41">
         <v>6</v>
@@ -2439,10 +2473,10 @@
         <v>15</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" s="42">
         <v>1</v>
@@ -2468,7 +2502,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" s="38" t="s">
         <v>4</v>
@@ -2497,10 +2531,10 @@
         <v>16</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" s="43">
         <v>0.5</v>
@@ -2551,13 +2585,13 @@
     </row>
     <row r="38" spans="3:5">
       <c r="C38" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="E38" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="39" spans="3:5">
@@ -2637,10 +2671,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C21:K73"/>
+  <dimension ref="C21:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2651,6 +2685,7 @@
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="21" spans="3:11" ht="15.75" thickBot="1"/>
@@ -2764,7 +2799,7 @@
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="19" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="G27" s="4">
         <v>3</v>
@@ -2787,7 +2822,7 @@
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G28" s="4">
         <v>3</v>
@@ -2810,7 +2845,7 @@
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G29" s="4">
         <v>3</v>
@@ -2833,7 +2868,7 @@
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="16" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="G30" s="4">
         <v>3</v>
@@ -2856,7 +2891,7 @@
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31" s="22">
         <v>3</v>
@@ -2900,7 +2935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:11">
+    <row r="33" spans="3:13">
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -2911,25 +2946,25 @@
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
     </row>
-    <row r="34" spans="3:11" ht="24" thickBot="1">
+    <row r="34" spans="3:13" ht="24" thickBot="1">
       <c r="C34" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="3:11">
+    <row r="35" spans="3:13">
       <c r="C35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="G35" s="70">
         <v>41323</v>
@@ -2947,15 +2982,15 @@
         <v>41327</v>
       </c>
     </row>
-    <row r="36" spans="3:11">
+    <row r="36" spans="3:13">
       <c r="C36" s="64">
         <v>1</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="F36" s="4">
         <v>1</v>
@@ -2976,205 +3011,220 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="3:11">
+    <row r="37" spans="3:13">
       <c r="C37" s="64">
         <v>17</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F37" s="4">
         <v>1.5</v>
       </c>
       <c r="G37" s="4">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="H37" s="4">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="I37" s="4">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="J37" s="4">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="K37" s="48">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="38" spans="3:11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13">
       <c r="C38" s="64">
         <v>4</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>48</v>
+        <v>38</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="F38" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G38" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H38" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I38" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J38" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K38" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="3:11">
+        <v>0.5</v>
+      </c>
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" spans="3:13">
       <c r="C39" s="64">
         <v>5</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>3</v>
       </c>
       <c r="F39" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G39" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J39" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K39" s="48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="3:11">
+        <v>1</v>
+      </c>
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="3:13">
       <c r="C40" s="64">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>70</v>
+      </c>
       <c r="F40" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G40" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H40" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I40" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J40" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K40" s="48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="3:11">
+        <v>3</v>
+      </c>
+      <c r="M40" s="14"/>
+    </row>
+    <row r="41" spans="3:13">
       <c r="C41" s="72">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D41" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="E41" s="73"/>
+        <v>68</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>7</v>
+      </c>
       <c r="F41" s="73">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G41" s="73">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="H41" s="73">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I41" s="73">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="J41" s="73">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K41" s="74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="3:11">
+        <v>0.5</v>
+      </c>
+      <c r="M41" s="14"/>
+    </row>
+    <row r="42" spans="3:13">
       <c r="C42" s="65">
         <v>19</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="F42" s="26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G42" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" s="66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="3:11">
-      <c r="C43" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76">
-        <v>1</v>
-      </c>
-      <c r="G43" s="76">
-        <v>1</v>
-      </c>
-      <c r="H43" s="76">
-        <v>1</v>
-      </c>
-      <c r="I43" s="76">
-        <v>1</v>
-      </c>
-      <c r="J43" s="76">
-        <v>1</v>
-      </c>
-      <c r="K43" s="77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="3:11">
-      <c r="C44" s="75"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="14"/>
+    </row>
+    <row r="43" spans="3:13">
+      <c r="C43" s="72">
+        <v>23</v>
+      </c>
+      <c r="D43" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="G43" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="H43" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="I43" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="J43" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="K43" s="66">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13">
+      <c r="C44" s="75" t="s">
+        <v>64</v>
+      </c>
       <c r="D44" s="76" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E44" s="76"/>
       <c r="F44" s="76">
@@ -3196,10 +3246,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="3:11">
+    <row r="45" spans="3:13">
       <c r="C45" s="75"/>
       <c r="D45" s="76" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E45" s="76"/>
       <c r="F45" s="76">
@@ -3221,10 +3271,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="3:11">
+    <row r="46" spans="3:13">
       <c r="C46" s="75"/>
       <c r="D46" s="76" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E46" s="76"/>
       <c r="F46" s="76">
@@ -3246,10 +3296,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="3:11">
+    <row r="47" spans="3:13">
       <c r="C47" s="75"/>
       <c r="D47" s="76" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E47" s="76"/>
       <c r="F47" s="76">
@@ -3271,10 +3321,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="3:11">
+    <row r="48" spans="3:13">
       <c r="C48" s="75"/>
       <c r="D48" s="76" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E48" s="76"/>
       <c r="F48" s="76">
@@ -3299,7 +3349,7 @@
     <row r="49" spans="3:11">
       <c r="C49" s="75"/>
       <c r="D49" s="76" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E49" s="76"/>
       <c r="F49" s="76">
@@ -3324,7 +3374,7 @@
     <row r="50" spans="3:11">
       <c r="C50" s="75"/>
       <c r="D50" s="76" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E50" s="76"/>
       <c r="F50" s="76">
@@ -3349,7 +3399,7 @@
     <row r="51" spans="3:11">
       <c r="C51" s="75"/>
       <c r="D51" s="76" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E51" s="76"/>
       <c r="F51" s="76">
@@ -3374,7 +3424,7 @@
     <row r="52" spans="3:11">
       <c r="C52" s="75"/>
       <c r="D52" s="76" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E52" s="76"/>
       <c r="F52" s="76">
@@ -3399,7 +3449,7 @@
     <row r="53" spans="3:11">
       <c r="C53" s="75"/>
       <c r="D53" s="76" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E53" s="76"/>
       <c r="F53" s="76">
@@ -3424,7 +3474,7 @@
     <row r="54" spans="3:11">
       <c r="C54" s="75"/>
       <c r="D54" s="76" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E54" s="76"/>
       <c r="F54" s="76">
@@ -3449,7 +3499,7 @@
     <row r="55" spans="3:11">
       <c r="C55" s="75"/>
       <c r="D55" s="76" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E55" s="76"/>
       <c r="F55" s="76">
@@ -3474,7 +3524,7 @@
     <row r="56" spans="3:11">
       <c r="C56" s="75"/>
       <c r="D56" s="76" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E56" s="76"/>
       <c r="F56" s="76">
@@ -3499,7 +3549,7 @@
     <row r="57" spans="3:11">
       <c r="C57" s="75"/>
       <c r="D57" s="76" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E57" s="76"/>
       <c r="F57" s="76">
@@ -3521,66 +3571,91 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="3:11" ht="15.75" thickBot="1">
-      <c r="C58" s="78"/>
-      <c r="D58" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="E58" s="79"/>
-      <c r="F58" s="79">
-        <v>1</v>
-      </c>
-      <c r="G58" s="79">
-        <v>1</v>
-      </c>
-      <c r="H58" s="79">
-        <v>1</v>
-      </c>
-      <c r="I58" s="79">
-        <v>1</v>
-      </c>
-      <c r="J58" s="79">
-        <v>1</v>
-      </c>
-      <c r="K58" s="80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="3:11">
-      <c r="F59" s="10">
-        <f>SUM(F36:F58)</f>
-        <v>26.5</v>
-      </c>
-      <c r="G59" s="14">
-        <f t="shared" ref="G59:K59" si="0">SUM(G36:G58)</f>
-        <v>26.5</v>
-      </c>
-      <c r="H59" s="14">
-        <f t="shared" si="0"/>
-        <v>26.5</v>
-      </c>
-      <c r="I59" s="14">
-        <f t="shared" si="0"/>
-        <v>26.5</v>
-      </c>
-      <c r="J59" s="14">
-        <f t="shared" si="0"/>
-        <v>26.5</v>
-      </c>
-      <c r="K59" s="14">
-        <f t="shared" si="0"/>
-        <v>26.5</v>
+    <row r="58" spans="3:11">
+      <c r="C58" s="75"/>
+      <c r="D58" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="E58" s="76"/>
+      <c r="F58" s="76">
+        <v>1</v>
+      </c>
+      <c r="G58" s="76">
+        <v>1</v>
+      </c>
+      <c r="H58" s="76">
+        <v>1</v>
+      </c>
+      <c r="I58" s="76">
+        <v>1</v>
+      </c>
+      <c r="J58" s="76">
+        <v>1</v>
+      </c>
+      <c r="K58" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" ht="15.75" thickBot="1">
+      <c r="C59" s="78"/>
+      <c r="D59" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="E59" s="79"/>
+      <c r="F59" s="79">
+        <v>1</v>
+      </c>
+      <c r="G59" s="79">
+        <v>1</v>
+      </c>
+      <c r="H59" s="79">
+        <v>1</v>
+      </c>
+      <c r="I59" s="79">
+        <v>1</v>
+      </c>
+      <c r="J59" s="79">
+        <v>1</v>
+      </c>
+      <c r="K59" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11">
+      <c r="F60" s="10">
+        <f>SUM(F36:F59)</f>
+        <v>24.5</v>
+      </c>
+      <c r="G60" s="14">
+        <f>SUM(G36:G59)</f>
+        <v>23</v>
+      </c>
+      <c r="H60" s="14">
+        <f>SUM(H36:H59)</f>
+        <v>23</v>
+      </c>
+      <c r="I60" s="14">
+        <f>SUM(I36:I59)</f>
+        <v>23</v>
+      </c>
+      <c r="J60" s="14">
+        <f>SUM(J36:J59)</f>
+        <v>23</v>
+      </c>
+      <c r="K60" s="14">
+        <f>SUM(K36:K59)</f>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="3:5">
       <c r="C68" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D68" s="14" t="s">
+      <c r="E68" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="E68" s="14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="69" spans="3:5">
@@ -3592,8 +3667,8 @@
         <v>24</v>
       </c>
       <c r="E69" s="14">
-        <f>G59</f>
-        <v>26.5</v>
+        <f>G60</f>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="3:5">
@@ -3605,8 +3680,8 @@
         <v>20</v>
       </c>
       <c r="E70" s="14">
-        <f>H59</f>
-        <v>26.5</v>
+        <f>H60</f>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="3:5">
@@ -3618,8 +3693,8 @@
         <v>12</v>
       </c>
       <c r="E71" s="14">
-        <f>I59</f>
-        <v>26.5</v>
+        <f>I60</f>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="3:5">
@@ -3631,8 +3706,8 @@
         <v>8</v>
       </c>
       <c r="E72" s="14">
-        <f>J59</f>
-        <v>26.5</v>
+        <f>J60</f>
+        <v>23</v>
       </c>
     </row>
     <row r="73" spans="3:5">
@@ -3644,8 +3719,8 @@
         <v>0</v>
       </c>
       <c r="E73" s="14">
-        <f>K59</f>
-        <v>26.5</v>
+        <f>K60</f>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored and created general menu
Signed-off-by: Christoffer Johnsson <stoffe1992@hotmail.com>
</commit_message>
<xml_diff>
--- a/doc/Game BurnDownChart.xlsx
+++ b/doc/Game BurnDownChart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
   <si>
     <t>Resouces</t>
   </si>
@@ -231,7 +231,10 @@
     <t>Alla</t>
   </si>
   <si>
-    <t>Skriva in i XNA</t>
+    <t>Skriva in sitt namn</t>
+  </si>
+  <si>
+    <t>Tobias/Stoffe</t>
   </si>
 </sst>
 </file>
@@ -1026,25 +1029,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95438336"/>
-        <c:axId val="95439872"/>
+        <c:axId val="82134528"/>
+        <c:axId val="82136064"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="95438336"/>
+        <c:axId val="82134528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95439872"/>
+        <c:crossAx val="82136064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="95439872"/>
+        <c:axId val="82136064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1052,7 +1055,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95438336"/>
+        <c:crossAx val="82134528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1063,8 +1066,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.70358202099737399"/>
-          <c:y val="0.43017169728784038"/>
+          <c:x val="0.70358202099737388"/>
+          <c:y val="0.43017169728784049"/>
           <c:w val="0.28934631459510268"/>
           <c:h val="0.31366825900341838"/>
         </c:manualLayout>
@@ -1075,7 +1078,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1091,8 +1094,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.0652066016912558E-2"/>
-          <c:y val="8.9589878188303523E-2"/>
+          <c:x val="9.0652066016912572E-2"/>
+          <c:y val="8.9589878188303537E-2"/>
           <c:w val="0.50605584698953865"/>
           <c:h val="0.64173685981560002"/>
         </c:manualLayout>
@@ -1213,44 +1216,44 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95645056"/>
-        <c:axId val="95663232"/>
+        <c:axId val="82484608"/>
+        <c:axId val="82494592"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="95645056"/>
+        <c:axId val="82484608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95663232"/>
+        <c:crossAx val="82494592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="95663232"/>
+        <c:axId val="82494592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,7 +1261,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95645056"/>
+        <c:crossAx val="82484608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1271,7 +1274,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2673,7 +2676,7 @@
   <dimension ref="C21:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2995,19 +2998,19 @@
         <v>1</v>
       </c>
       <c r="G36" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H36" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I36" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J36" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K36" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="3:13">
@@ -3021,10 +3024,10 @@
         <v>46</v>
       </c>
       <c r="F37" s="4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G37" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H37" s="4">
         <v>0</v>
@@ -3053,19 +3056,19 @@
         <v>0.5</v>
       </c>
       <c r="G38" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H38" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I38" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J38" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K38" s="48">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M38" s="14"/>
     </row>
@@ -3197,25 +3200,25 @@
         <v>71</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="F43" s="69">
         <v>0.5</v>
       </c>
       <c r="G43" s="69">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H43" s="69">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I43" s="69">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J43" s="69">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K43" s="66">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="3:13">
@@ -3623,27 +3626,27 @@
     <row r="60" spans="3:11">
       <c r="F60" s="10">
         <f t="shared" ref="F60:K60" si="0">SUM(F36:F59)</f>
-        <v>24.5</v>
+        <v>24</v>
       </c>
       <c r="G60" s="14">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H60" s="14">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>20</v>
       </c>
       <c r="I60" s="14">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>20</v>
       </c>
       <c r="J60" s="14">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>20</v>
       </c>
       <c r="K60" s="14">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="3:5">
@@ -3667,7 +3670,7 @@
       </c>
       <c r="E69" s="14">
         <f>G60</f>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="3:5">
@@ -3680,7 +3683,7 @@
       </c>
       <c r="E70" s="14">
         <f>H60</f>
-        <v>21.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="3:5">
@@ -3693,7 +3696,7 @@
       </c>
       <c r="E71" s="14">
         <f>I60</f>
-        <v>21.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="3:5">
@@ -3706,7 +3709,7 @@
       </c>
       <c r="E72" s="14">
         <f>J60</f>
-        <v>21.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="3:5">
@@ -3719,7 +3722,7 @@
       </c>
       <c r="E73" s="14">
         <f>K60</f>
-        <v>21.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>